<commit_message>
Updated Blog and import+export required changes for blog
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/sample_import_template_with_guide.xlsx
+++ b/src/main/resources/templates/sample_import_template_with_guide.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7308" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="IMPORT_GUIDE" sheetId="1" r:id="rId1"/>
@@ -23,12 +18,12 @@
     <sheet name="PartnerRequests" sheetId="9" r:id="rId9"/>
     <sheet name="Subscribers" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
   <si>
     <t>This Excel file is structured to help you import website data easily.</t>
   </si>
@@ -120,24 +115,12 @@
     <t>industry</t>
   </si>
   <si>
-    <t>subtitle</t>
-  </si>
-  <si>
     <t>authorName</t>
   </si>
   <si>
     <t>content</t>
   </si>
   <si>
-    <t>advantages</t>
-  </si>
-  <si>
-    <t>disadvantages</t>
-  </si>
-  <si>
-    <t>conclusion</t>
-  </si>
-  <si>
     <t>subject</t>
   </si>
   <si>
@@ -1143,13 +1126,28 @@
   </si>
   <si>
     <t>subheading</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>publish</t>
+  </si>
+  <si>
+    <t>bannerUrl</t>
+  </si>
+  <si>
+    <t>serpTitle</t>
+  </si>
+  <si>
+    <t>serpMetaDescription</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1328,7 +1326,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1360,10 +1358,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1395,7 +1392,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1571,408 +1567,408 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A79"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="E80" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18">
       <c r="A1" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="17.399999999999999">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="17.399999999999999">
+      <c r="A10" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="17" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+    <row r="44" spans="1:1">
+      <c r="A44" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+    <row r="54" spans="1:1">
+      <c r="A54" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+    <row r="57" spans="1:1">
+      <c r="A57" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+    <row r="62" spans="1:1">
+      <c r="A62" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+    <row r="74" spans="1:1">
+      <c r="A74" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+    <row r="76" spans="1:1">
+      <c r="A76" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+    <row r="77" spans="1:1">
+      <c r="A77" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" s="6" t="s">
+    <row r="79" spans="1:1">
+      <c r="A79" s="6" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A79" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1982,16 +1978,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2002,36 +1998,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="D2" s="7"/>
     </row>
   </sheetData>
@@ -2041,21 +2037,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2063,13 +2059,13 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2078,30 +2074,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="4" max="4" width="20.90625" customWidth="1"/>
-    <col min="5" max="5" width="24.81640625" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" customWidth="1"/>
-    <col min="9" max="9" width="23.6328125" customWidth="1"/>
-    <col min="10" max="10" width="23.453125" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" customWidth="1"/>
-    <col min="12" max="12" width="20.54296875" customWidth="1"/>
-    <col min="13" max="13" width="16.81640625" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" customWidth="1"/>
+    <col min="12" max="12" width="20.5546875" customWidth="1"/>
+    <col min="13" max="13" width="16.77734375" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2151,16 +2147,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2183,36 +2179,36 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="19.6328125" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" customWidth="1"/>
-    <col min="7" max="7" width="24.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>26</v>
@@ -2233,52 +2229,50 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="14.26953125" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" customWidth="1"/>
-    <col min="8" max="8" width="23.08984375" customWidth="1"/>
-    <col min="9" max="9" width="16.90625" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="J1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2286,16 +2280,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2303,13 +2297,13 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>23</v>
@@ -2318,7 +2312,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2327,21 +2321,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
@@ -2350,7 +2344,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
import,export serviceImpl fileds update accoridng to new  service variables
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/sample_import_template_with_guide.xlsx
+++ b/src/main/resources/templates/sample_import_template_with_guide.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7308" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7308" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IMPORT_GUIDE" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="114">
   <si>
     <t>This Excel file is structured to help you import website data easily.</t>
   </si>
@@ -1141,6 +1141,15 @@
   </si>
   <si>
     <t>serpMetaDescription</t>
+  </si>
+  <si>
+    <t>metaTitle</t>
+  </si>
+  <si>
+    <t>metaDescription</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -1999,10 +2008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2010,24 +2019,36 @@
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1">
+    <row r="1" spans="1:9" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="F1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:9">
       <c r="D2" s="7"/>
     </row>
   </sheetData>
@@ -2232,7 +2253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>

</xml_diff>